<commit_message>
Enable to use original App component with CommunicationController.
</commit_message>
<xml_diff>
--- a/meta/components/CommunicationController.xlsx
+++ b/meta/components/CommunicationController.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/dapanda/dapanda-front-core/meta/components/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88F6913A-3D24-0E4E-A37E-3AC1BC63D1BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3F5424E0-96DF-1342-8570-2D6D0C00983F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2700" yWindow="1880" windowWidth="25200" windowHeight="17540" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1540" yWindow="6160" windowWidth="25200" windowHeight="17540" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="VueComponent" sheetId="1" r:id="rId1"/>
@@ -37,6 +37,7 @@
     <definedName name="必須">#REF!</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -57,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="101">
   <si>
     <t>パッケージ</t>
   </si>
@@ -846,6 +847,81 @@
     <rPh sb="3" eb="5">
       <t xml:space="preserve">セイギョ </t>
     </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>appComponent</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>{}</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>CommunicationController 配下に置く App コンポーネントを指定します。</t>
+    <rPh sb="24" eb="26">
+      <t xml:space="preserve">ハイカニ </t>
+    </rPh>
+    <rPh sb="27" eb="28">
+      <t xml:space="preserve">オク </t>
+    </rPh>
+    <rPh sb="42" eb="44">
+      <t xml:space="preserve">シテイ </t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>nopagePath</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>DefineComponent</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>import { DefineComponent } from "vue"</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>noAuthPath</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>ページが存在しなかった場合のrouteを指定染ます。Appコンポーネントに渡します。</t>
+    <rPh sb="4" eb="6">
+      <t xml:space="preserve">ソンザイ </t>
+    </rPh>
+    <rPh sb="11" eb="13">
+      <t xml:space="preserve">バアイノ </t>
+    </rPh>
+    <rPh sb="20" eb="23">
+      <t xml:space="preserve">シテイシマス。 </t>
+    </rPh>
+    <rPh sb="37" eb="38">
+      <t xml:space="preserve">ワタシマス シテイシマス。 </t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>認証に失敗した場合のrouteを指定染ます。Appコンポーネントに渡します。</t>
+    <rPh sb="0" eb="2">
+      <t xml:space="preserve">ニンンショウニ </t>
+    </rPh>
+    <rPh sb="3" eb="5">
+      <t xml:space="preserve">シッパイ </t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>"/nopageSample"</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>"/login"</t>
     <phoneticPr fontId="3"/>
   </si>
 </sst>
@@ -1657,6 +1733,45 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1665,45 +1780,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2118,8 +2194,8 @@
   </sheetPr>
   <dimension ref="A1:M97"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="E65" sqref="E65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -2234,10 +2310,10 @@
       <c r="I9" s="35"/>
     </row>
     <row r="10" spans="1:11">
-      <c r="A10" s="101" t="s">
+      <c r="A10" s="102" t="s">
         <v>44</v>
       </c>
-      <c r="B10" s="102"/>
+      <c r="B10" s="103"/>
       <c r="C10" s="10"/>
       <c r="D10" s="33"/>
       <c r="E10" s="11"/>
@@ -2249,10 +2325,10 @@
       <c r="I10" s="35"/>
     </row>
     <row r="11" spans="1:11">
-      <c r="A11" s="101" t="s">
+      <c r="A11" s="102" t="s">
         <v>45</v>
       </c>
-      <c r="B11" s="102"/>
+      <c r="B11" s="103"/>
       <c r="C11" s="10"/>
       <c r="D11" s="33"/>
       <c r="E11" s="11"/>
@@ -2264,10 +2340,10 @@
       <c r="I11" s="35"/>
     </row>
     <row r="12" spans="1:11">
-      <c r="A12" s="101" t="s">
+      <c r="A12" s="102" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="102"/>
+      <c r="B12" s="103"/>
       <c r="C12" s="10" t="s">
         <v>21</v>
       </c>
@@ -2281,10 +2357,10 @@
       <c r="I12" s="35"/>
     </row>
     <row r="13" spans="1:11">
-      <c r="A13" s="101" t="s">
+      <c r="A13" s="102" t="s">
         <v>39</v>
       </c>
-      <c r="B13" s="102"/>
+      <c r="B13" s="103"/>
       <c r="C13" s="86" t="s">
         <v>48</v>
       </c>
@@ -2302,11 +2378,11 @@
         <v>1</v>
       </c>
       <c r="B14" s="6"/>
-      <c r="C14" s="103" t="s">
+      <c r="C14" s="104" t="s">
         <v>88</v>
       </c>
-      <c r="D14" s="104"/>
-      <c r="E14" s="105"/>
+      <c r="D14" s="105"/>
+      <c r="E14" s="106"/>
       <c r="F14" s="65"/>
       <c r="G14" s="65"/>
       <c r="H14" s="65"/>
@@ -2443,10 +2519,10 @@
       <c r="I22"/>
     </row>
     <row r="23" spans="1:13" s="32" customFormat="1">
-      <c r="A23" s="106" t="s">
+      <c r="A23" s="94" t="s">
         <v>60</v>
       </c>
-      <c r="B23" s="107"/>
+      <c r="B23" s="95"/>
       <c r="C23" s="64"/>
       <c r="D23" t="s">
         <v>58</v>
@@ -2473,10 +2549,10 @@
       <c r="I24"/>
     </row>
     <row r="25" spans="1:13" s="32" customFormat="1">
-      <c r="A25" s="106" t="s">
+      <c r="A25" s="94" t="s">
         <v>18</v>
       </c>
-      <c r="B25" s="107"/>
+      <c r="B25" s="95"/>
       <c r="C25" s="64" t="s">
         <v>14</v>
       </c>
@@ -2490,10 +2566,10 @@
       <c r="I25"/>
     </row>
     <row r="26" spans="1:13" s="32" customFormat="1">
-      <c r="A26" s="106" t="s">
+      <c r="A26" s="94" t="s">
         <v>49</v>
       </c>
-      <c r="B26" s="107"/>
+      <c r="B26" s="95"/>
       <c r="C26" s="64" t="s">
         <v>14</v>
       </c>
@@ -2948,8 +3024,12 @@
       <c r="M53" s="35"/>
     </row>
     <row r="54" spans="1:13">
-      <c r="A54" s="51"/>
-      <c r="B54" s="46"/>
+      <c r="A54" s="51">
+        <v>1</v>
+      </c>
+      <c r="B54" s="46" t="s">
+        <v>95</v>
+      </c>
       <c r="C54" s="38"/>
       <c r="D54" s="38"/>
       <c r="E54" s="39"/>
@@ -3036,49 +3116,49 @@
       <c r="M59" s="15"/>
     </row>
     <row r="60" spans="1:13" ht="13.5" customHeight="1">
-      <c r="A60" s="100" t="s">
+      <c r="A60" s="97" t="s">
         <v>7</v>
       </c>
-      <c r="B60" s="100" t="s">
+      <c r="B60" s="97" t="s">
         <v>3</v>
       </c>
-      <c r="C60" s="97" t="s">
+      <c r="C60" s="96" t="s">
         <v>4</v>
       </c>
-      <c r="D60" s="97" t="s">
+      <c r="D60" s="96" t="s">
         <v>6</v>
       </c>
-      <c r="E60" s="97" t="s">
+      <c r="E60" s="96" t="s">
         <v>5</v>
       </c>
-      <c r="F60" s="98" t="s">
+      <c r="F60" s="100" t="s">
         <v>33</v>
       </c>
-      <c r="G60" s="98" t="s">
+      <c r="G60" s="100" t="s">
         <v>16</v>
       </c>
-      <c r="H60" s="108" t="s">
+      <c r="H60" s="98" t="s">
         <v>81</v>
       </c>
-      <c r="I60" s="97" t="s">
+      <c r="I60" s="96" t="s">
         <v>1</v>
       </c>
-      <c r="J60" s="97"/>
+      <c r="J60" s="96"/>
       <c r="K60" s="16"/>
       <c r="L60" s="17"/>
       <c r="M60" s="9"/>
     </row>
     <row r="61" spans="1:13">
-      <c r="A61" s="100"/>
-      <c r="B61" s="100"/>
-      <c r="C61" s="97"/>
-      <c r="D61" s="97"/>
-      <c r="E61" s="97"/>
-      <c r="F61" s="99"/>
-      <c r="G61" s="99"/>
-      <c r="H61" s="109"/>
-      <c r="I61" s="97"/>
-      <c r="J61" s="97"/>
+      <c r="A61" s="97"/>
+      <c r="B61" s="97"/>
+      <c r="C61" s="96"/>
+      <c r="D61" s="96"/>
+      <c r="E61" s="96"/>
+      <c r="F61" s="101"/>
+      <c r="G61" s="101"/>
+      <c r="H61" s="99"/>
+      <c r="I61" s="96"/>
+      <c r="J61" s="96"/>
       <c r="K61" s="18"/>
       <c r="L61" s="29"/>
       <c r="M61" s="15"/>
@@ -3087,14 +3167,24 @@
       <c r="A62" s="19">
         <v>1</v>
       </c>
-      <c r="B62" s="71"/>
-      <c r="C62" s="78"/>
+      <c r="B62" s="71" t="s">
+        <v>89</v>
+      </c>
+      <c r="C62" s="78" t="s">
+        <v>94</v>
+      </c>
       <c r="D62" s="20"/>
-      <c r="E62" s="20"/>
-      <c r="F62" s="20"/>
+      <c r="E62" s="20" t="s">
+        <v>90</v>
+      </c>
+      <c r="F62" s="20" t="s">
+        <v>14</v>
+      </c>
       <c r="G62" s="69"/>
       <c r="H62" s="69"/>
-      <c r="I62" s="20"/>
+      <c r="I62" s="20" t="s">
+        <v>91</v>
+      </c>
       <c r="J62" s="21"/>
       <c r="K62" s="21"/>
       <c r="L62" s="28"/>
@@ -3105,14 +3195,22 @@
         <f>A62+1</f>
         <v>2</v>
       </c>
-      <c r="B63" s="71"/>
-      <c r="C63" s="78"/>
+      <c r="B63" s="71" t="s">
+        <v>92</v>
+      </c>
+      <c r="C63" s="78" t="s">
+        <v>93</v>
+      </c>
       <c r="D63" s="20"/>
-      <c r="E63" s="20"/>
+      <c r="E63" s="20" t="s">
+        <v>99</v>
+      </c>
       <c r="F63" s="20"/>
       <c r="G63" s="69"/>
       <c r="H63" s="69"/>
-      <c r="I63" s="20"/>
+      <c r="I63" s="20" t="s">
+        <v>97</v>
+      </c>
       <c r="J63" s="21"/>
       <c r="K63" s="21"/>
       <c r="L63" s="28"/>
@@ -3123,14 +3221,22 @@
         <f t="shared" ref="A64:A78" si="0">A63+1</f>
         <v>3</v>
       </c>
-      <c r="B64" s="72"/>
-      <c r="C64" s="79"/>
+      <c r="B64" s="72" t="s">
+        <v>96</v>
+      </c>
+      <c r="C64" s="79" t="s">
+        <v>93</v>
+      </c>
       <c r="D64" s="20"/>
-      <c r="E64" s="20"/>
+      <c r="E64" s="20" t="s">
+        <v>100</v>
+      </c>
       <c r="F64" s="20"/>
       <c r="G64" s="69"/>
       <c r="H64" s="69"/>
-      <c r="I64" s="20"/>
+      <c r="I64" s="20" t="s">
+        <v>98</v>
+      </c>
       <c r="J64" s="21"/>
       <c r="K64" s="21"/>
       <c r="L64" s="22"/>
@@ -3530,41 +3636,41 @@
       <c r="M88" s="15"/>
     </row>
     <row r="89" spans="1:13" ht="13.5" customHeight="1">
-      <c r="A89" s="100" t="s">
+      <c r="A89" s="97" t="s">
         <v>7</v>
       </c>
-      <c r="B89" s="100" t="s">
+      <c r="B89" s="97" t="s">
         <v>68</v>
       </c>
-      <c r="C89" s="97" t="s">
+      <c r="C89" s="96" t="s">
         <v>70</v>
       </c>
-      <c r="D89" s="97" t="s">
+      <c r="D89" s="96" t="s">
         <v>71</v>
       </c>
-      <c r="E89" s="97" t="s">
+      <c r="E89" s="96" t="s">
         <v>65</v>
       </c>
-      <c r="F89" s="94"/>
-      <c r="G89" s="94"/>
-      <c r="H89" s="94"/>
-      <c r="I89" s="96"/>
-      <c r="J89" s="97"/>
+      <c r="F89" s="107"/>
+      <c r="G89" s="107"/>
+      <c r="H89" s="107"/>
+      <c r="I89" s="109"/>
+      <c r="J89" s="96"/>
       <c r="K89" s="16"/>
       <c r="L89" s="17"/>
       <c r="M89" s="9"/>
     </row>
     <row r="90" spans="1:13">
-      <c r="A90" s="100"/>
-      <c r="B90" s="100"/>
-      <c r="C90" s="97"/>
-      <c r="D90" s="97"/>
-      <c r="E90" s="97"/>
-      <c r="F90" s="95"/>
-      <c r="G90" s="95"/>
-      <c r="H90" s="95"/>
-      <c r="I90" s="96"/>
-      <c r="J90" s="97"/>
+      <c r="A90" s="97"/>
+      <c r="B90" s="97"/>
+      <c r="C90" s="96"/>
+      <c r="D90" s="96"/>
+      <c r="E90" s="96"/>
+      <c r="F90" s="108"/>
+      <c r="G90" s="108"/>
+      <c r="H90" s="108"/>
+      <c r="I90" s="109"/>
+      <c r="J90" s="96"/>
       <c r="K90" s="18"/>
       <c r="L90" s="29"/>
       <c r="M90" s="15"/>
@@ -3696,6 +3802,21 @@
     </row>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="F89:F90"/>
+    <mergeCell ref="H89:H90"/>
+    <mergeCell ref="I89:J90"/>
+    <mergeCell ref="G60:G61"/>
+    <mergeCell ref="G89:G90"/>
+    <mergeCell ref="A89:A90"/>
+    <mergeCell ref="B89:B90"/>
+    <mergeCell ref="C89:C90"/>
+    <mergeCell ref="D89:D90"/>
+    <mergeCell ref="E89:E90"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="C14:E14"/>
     <mergeCell ref="A25:B25"/>
     <mergeCell ref="A23:B23"/>
     <mergeCell ref="I60:J61"/>
@@ -3707,21 +3828,6 @@
     <mergeCell ref="H60:H61"/>
     <mergeCell ref="F60:F61"/>
     <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="C14:E14"/>
-    <mergeCell ref="A89:A90"/>
-    <mergeCell ref="B89:B90"/>
-    <mergeCell ref="C89:C90"/>
-    <mergeCell ref="D89:D90"/>
-    <mergeCell ref="E89:E90"/>
-    <mergeCell ref="F89:F90"/>
-    <mergeCell ref="H89:H90"/>
-    <mergeCell ref="I89:J90"/>
-    <mergeCell ref="G60:G61"/>
-    <mergeCell ref="G89:G90"/>
   </mergeCells>
   <phoneticPr fontId="3"/>
   <dataValidations count="5">

</xml_diff>

<commit_message>
Enable select authentication header.
</commit_message>
<xml_diff>
--- a/meta/components/CommunicationController.xlsx
+++ b/meta/components/CommunicationController.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11011"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/dapanda/dapanda-front-core/meta/components/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3F5424E0-96DF-1342-8570-2D6D0C00983F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8A43AC3-FA30-5C40-92F1-1C591A58217D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1540" yWindow="6160" windowWidth="25200" windowHeight="17540" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1540" yWindow="500" windowWidth="25200" windowHeight="17500" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="VueComponent" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,6 @@
     <definedName name="必須">#REF!</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -58,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="107">
   <si>
     <t>パッケージ</t>
   </si>
@@ -922,6 +921,42 @@
   </si>
   <si>
     <t>"/login"</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>authHeader</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>"X-Dapanda-AccessToken"</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>認証トークンを保持する HTTP ヘッダです。</t>
+    <rPh sb="0" eb="1">
+      <t xml:space="preserve">ニンショウ </t>
+    </rPh>
+    <rPh sb="7" eb="9">
+      <t xml:space="preserve">ホジスル </t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>useBearer</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>boolean</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>認可トークンに Bearer を付与するかどうか。</t>
+    <rPh sb="0" eb="2">
+      <t xml:space="preserve">ニンカ </t>
+    </rPh>
+    <rPh sb="16" eb="18">
+      <t xml:space="preserve">フヨスルカ </t>
+    </rPh>
     <phoneticPr fontId="3"/>
   </si>
 </sst>
@@ -1733,53 +1768,53 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2195,7 +2230,7 @@
   <dimension ref="A1:M97"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="E65" sqref="E65"/>
+      <selection activeCell="I67" sqref="I67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -2310,10 +2345,10 @@
       <c r="I9" s="35"/>
     </row>
     <row r="10" spans="1:11">
-      <c r="A10" s="102" t="s">
+      <c r="A10" s="101" t="s">
         <v>44</v>
       </c>
-      <c r="B10" s="103"/>
+      <c r="B10" s="102"/>
       <c r="C10" s="10"/>
       <c r="D10" s="33"/>
       <c r="E10" s="11"/>
@@ -2325,10 +2360,10 @@
       <c r="I10" s="35"/>
     </row>
     <row r="11" spans="1:11">
-      <c r="A11" s="102" t="s">
+      <c r="A11" s="101" t="s">
         <v>45</v>
       </c>
-      <c r="B11" s="103"/>
+      <c r="B11" s="102"/>
       <c r="C11" s="10"/>
       <c r="D11" s="33"/>
       <c r="E11" s="11"/>
@@ -2340,10 +2375,10 @@
       <c r="I11" s="35"/>
     </row>
     <row r="12" spans="1:11">
-      <c r="A12" s="102" t="s">
+      <c r="A12" s="101" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="103"/>
+      <c r="B12" s="102"/>
       <c r="C12" s="10" t="s">
         <v>21</v>
       </c>
@@ -2357,10 +2392,10 @@
       <c r="I12" s="35"/>
     </row>
     <row r="13" spans="1:11">
-      <c r="A13" s="102" t="s">
+      <c r="A13" s="101" t="s">
         <v>39</v>
       </c>
-      <c r="B13" s="103"/>
+      <c r="B13" s="102"/>
       <c r="C13" s="86" t="s">
         <v>48</v>
       </c>
@@ -2378,11 +2413,11 @@
         <v>1</v>
       </c>
       <c r="B14" s="6"/>
-      <c r="C14" s="104" t="s">
+      <c r="C14" s="103" t="s">
         <v>88</v>
       </c>
-      <c r="D14" s="105"/>
-      <c r="E14" s="106"/>
+      <c r="D14" s="104"/>
+      <c r="E14" s="105"/>
       <c r="F14" s="65"/>
       <c r="G14" s="65"/>
       <c r="H14" s="65"/>
@@ -2519,10 +2554,10 @@
       <c r="I22"/>
     </row>
     <row r="23" spans="1:13" s="32" customFormat="1">
-      <c r="A23" s="94" t="s">
+      <c r="A23" s="106" t="s">
         <v>60</v>
       </c>
-      <c r="B23" s="95"/>
+      <c r="B23" s="107"/>
       <c r="C23" s="64"/>
       <c r="D23" t="s">
         <v>58</v>
@@ -2549,10 +2584,10 @@
       <c r="I24"/>
     </row>
     <row r="25" spans="1:13" s="32" customFormat="1">
-      <c r="A25" s="94" t="s">
+      <c r="A25" s="106" t="s">
         <v>18</v>
       </c>
-      <c r="B25" s="95"/>
+      <c r="B25" s="107"/>
       <c r="C25" s="64" t="s">
         <v>14</v>
       </c>
@@ -2566,10 +2601,10 @@
       <c r="I25"/>
     </row>
     <row r="26" spans="1:13" s="32" customFormat="1">
-      <c r="A26" s="94" t="s">
+      <c r="A26" s="106" t="s">
         <v>49</v>
       </c>
-      <c r="B26" s="95"/>
+      <c r="B26" s="107"/>
       <c r="C26" s="64" t="s">
         <v>14</v>
       </c>
@@ -3116,49 +3151,49 @@
       <c r="M59" s="15"/>
     </row>
     <row r="60" spans="1:13" ht="13.5" customHeight="1">
-      <c r="A60" s="97" t="s">
+      <c r="A60" s="100" t="s">
         <v>7</v>
       </c>
-      <c r="B60" s="97" t="s">
+      <c r="B60" s="100" t="s">
         <v>3</v>
       </c>
-      <c r="C60" s="96" t="s">
+      <c r="C60" s="97" t="s">
         <v>4</v>
       </c>
-      <c r="D60" s="96" t="s">
+      <c r="D60" s="97" t="s">
         <v>6</v>
       </c>
-      <c r="E60" s="96" t="s">
+      <c r="E60" s="97" t="s">
         <v>5</v>
       </c>
-      <c r="F60" s="100" t="s">
+      <c r="F60" s="98" t="s">
         <v>33</v>
       </c>
-      <c r="G60" s="100" t="s">
+      <c r="G60" s="98" t="s">
         <v>16</v>
       </c>
-      <c r="H60" s="98" t="s">
+      <c r="H60" s="108" t="s">
         <v>81</v>
       </c>
-      <c r="I60" s="96" t="s">
+      <c r="I60" s="97" t="s">
         <v>1</v>
       </c>
-      <c r="J60" s="96"/>
+      <c r="J60" s="97"/>
       <c r="K60" s="16"/>
       <c r="L60" s="17"/>
       <c r="M60" s="9"/>
     </row>
     <row r="61" spans="1:13">
-      <c r="A61" s="97"/>
-      <c r="B61" s="97"/>
-      <c r="C61" s="96"/>
-      <c r="D61" s="96"/>
-      <c r="E61" s="96"/>
-      <c r="F61" s="101"/>
-      <c r="G61" s="101"/>
-      <c r="H61" s="99"/>
-      <c r="I61" s="96"/>
-      <c r="J61" s="96"/>
+      <c r="A61" s="100"/>
+      <c r="B61" s="100"/>
+      <c r="C61" s="97"/>
+      <c r="D61" s="97"/>
+      <c r="E61" s="97"/>
+      <c r="F61" s="99"/>
+      <c r="G61" s="99"/>
+      <c r="H61" s="109"/>
+      <c r="I61" s="97"/>
+      <c r="J61" s="97"/>
       <c r="K61" s="18"/>
       <c r="L61" s="29"/>
       <c r="M61" s="15"/>
@@ -3247,14 +3282,22 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B65" s="73"/>
-      <c r="C65" s="80"/>
+      <c r="B65" s="73" t="s">
+        <v>101</v>
+      </c>
+      <c r="C65" s="80" t="s">
+        <v>93</v>
+      </c>
       <c r="D65" s="20"/>
-      <c r="E65" s="20"/>
+      <c r="E65" s="20" t="s">
+        <v>102</v>
+      </c>
       <c r="F65" s="20"/>
       <c r="G65" s="69"/>
       <c r="H65" s="69"/>
-      <c r="I65" s="20"/>
+      <c r="I65" s="20" t="s">
+        <v>103</v>
+      </c>
       <c r="J65" s="21"/>
       <c r="K65" s="21"/>
       <c r="L65" s="22"/>
@@ -3265,14 +3308,22 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B66" s="73"/>
-      <c r="C66" s="80"/>
+      <c r="B66" s="73" t="s">
+        <v>104</v>
+      </c>
+      <c r="C66" s="80" t="s">
+        <v>105</v>
+      </c>
       <c r="D66" s="20"/>
-      <c r="E66" s="20"/>
+      <c r="E66" s="20" t="b">
+        <v>0</v>
+      </c>
       <c r="F66" s="20"/>
       <c r="G66" s="69"/>
       <c r="H66" s="69"/>
-      <c r="I66" s="20"/>
+      <c r="I66" s="20" t="s">
+        <v>106</v>
+      </c>
       <c r="J66" s="21"/>
       <c r="K66" s="21"/>
       <c r="L66" s="22"/>
@@ -3636,41 +3687,41 @@
       <c r="M88" s="15"/>
     </row>
     <row r="89" spans="1:13" ht="13.5" customHeight="1">
-      <c r="A89" s="97" t="s">
+      <c r="A89" s="100" t="s">
         <v>7</v>
       </c>
-      <c r="B89" s="97" t="s">
+      <c r="B89" s="100" t="s">
         <v>68</v>
       </c>
-      <c r="C89" s="96" t="s">
+      <c r="C89" s="97" t="s">
         <v>70</v>
       </c>
-      <c r="D89" s="96" t="s">
+      <c r="D89" s="97" t="s">
         <v>71</v>
       </c>
-      <c r="E89" s="96" t="s">
+      <c r="E89" s="97" t="s">
         <v>65</v>
       </c>
-      <c r="F89" s="107"/>
-      <c r="G89" s="107"/>
-      <c r="H89" s="107"/>
-      <c r="I89" s="109"/>
-      <c r="J89" s="96"/>
+      <c r="F89" s="94"/>
+      <c r="G89" s="94"/>
+      <c r="H89" s="94"/>
+      <c r="I89" s="96"/>
+      <c r="J89" s="97"/>
       <c r="K89" s="16"/>
       <c r="L89" s="17"/>
       <c r="M89" s="9"/>
     </row>
     <row r="90" spans="1:13">
-      <c r="A90" s="97"/>
-      <c r="B90" s="97"/>
-      <c r="C90" s="96"/>
-      <c r="D90" s="96"/>
-      <c r="E90" s="96"/>
-      <c r="F90" s="108"/>
-      <c r="G90" s="108"/>
-      <c r="H90" s="108"/>
-      <c r="I90" s="109"/>
-      <c r="J90" s="96"/>
+      <c r="A90" s="100"/>
+      <c r="B90" s="100"/>
+      <c r="C90" s="97"/>
+      <c r="D90" s="97"/>
+      <c r="E90" s="97"/>
+      <c r="F90" s="95"/>
+      <c r="G90" s="95"/>
+      <c r="H90" s="95"/>
+      <c r="I90" s="96"/>
+      <c r="J90" s="97"/>
       <c r="K90" s="18"/>
       <c r="L90" s="29"/>
       <c r="M90" s="15"/>
@@ -3802,21 +3853,6 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="F89:F90"/>
-    <mergeCell ref="H89:H90"/>
-    <mergeCell ref="I89:J90"/>
-    <mergeCell ref="G60:G61"/>
-    <mergeCell ref="G89:G90"/>
-    <mergeCell ref="A89:A90"/>
-    <mergeCell ref="B89:B90"/>
-    <mergeCell ref="C89:C90"/>
-    <mergeCell ref="D89:D90"/>
-    <mergeCell ref="E89:E90"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="C14:E14"/>
     <mergeCell ref="A25:B25"/>
     <mergeCell ref="A23:B23"/>
     <mergeCell ref="I60:J61"/>
@@ -3828,6 +3864,21 @@
     <mergeCell ref="H60:H61"/>
     <mergeCell ref="F60:F61"/>
     <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="C14:E14"/>
+    <mergeCell ref="A89:A90"/>
+    <mergeCell ref="B89:B90"/>
+    <mergeCell ref="C89:C90"/>
+    <mergeCell ref="D89:D90"/>
+    <mergeCell ref="E89:E90"/>
+    <mergeCell ref="F89:F90"/>
+    <mergeCell ref="H89:H90"/>
+    <mergeCell ref="I89:J90"/>
+    <mergeCell ref="G60:G61"/>
+    <mergeCell ref="G89:G90"/>
   </mergeCells>
   <phoneticPr fontId="3"/>
   <dataValidations count="5">

</xml_diff>